<commit_message>
updated BOM with level shifter circuitry
</commit_message>
<xml_diff>
--- a/BOM/MEBv1.1_BOM.xlsx
+++ b/BOM/MEBv1.1_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\AD22\Projects\MEBv1\MEB\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CE3A43-DDD5-48D6-B887-F3DD7EA5622B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19F96BD-2ADF-4465-A70C-7368A345B3F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="450" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MEBv1.1_BOM" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,24 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">MEBv1.1_BOM!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="164">
   <si>
     <t>Designator</t>
   </si>
@@ -285,9 +297,6 @@
     <t>https://www.yageo.com/upload/media/product/productsearch/datasheet/rchip/PYu-RC_Group_51_RoHS_L_11.pdf</t>
   </si>
   <si>
-    <t>R2, R4, R11</t>
-  </si>
-  <si>
     <t>RES 10K OHM 5% 1/8W 0805</t>
   </si>
   <si>
@@ -339,9 +348,6 @@
     <t>RC0805FR-07140RL</t>
   </si>
   <si>
-    <t>R7</t>
-  </si>
-  <si>
     <t>RES 10 OHM 1% 1/8W 0805</t>
   </si>
   <si>
@@ -351,9 +357,6 @@
     <t>RC0805FR-0710RL</t>
   </si>
   <si>
-    <t>R8, R9, R10</t>
-  </si>
-  <si>
     <t>RES SMD 4.7K OHM 1% 1/8W 0805</t>
   </si>
   <si>
@@ -435,9 +438,6 @@
     <t>LED BLUE CLEAR 0805 SMD</t>
   </si>
   <si>
-    <t xml:space="preserve"> LED GREEN CLEAR 0805 SMD</t>
-  </si>
-  <si>
     <t>150080BS75000</t>
   </si>
   <si>
@@ -448,16 +448,118 @@
   </si>
   <si>
     <t>https://www.we-online.com/katalog/datasheet/150080GS75000.pdf</t>
+  </si>
+  <si>
+    <t>J1M</t>
+  </si>
+  <si>
+    <t>CONN RECEPT 10POS 3MM VERT DUAL</t>
+  </si>
+  <si>
+    <t>https://www.molex.com/pdm_docs/ps/PS-43045.pdf</t>
+  </si>
+  <si>
+    <t>J1MC</t>
+  </si>
+  <si>
+    <t>CONN SOCKET 20-24AWG CRIMP GOLD</t>
+  </si>
+  <si>
+    <t>https://www.molex.com/pdm_docs/ps/PS-44300-001.pdf</t>
+  </si>
+  <si>
+    <t>P1.1</t>
+  </si>
+  <si>
+    <t>SSQ-110-03-F-S</t>
+  </si>
+  <si>
+    <t>Samtec Inc.</t>
+  </si>
+  <si>
+    <t>P1.2</t>
+  </si>
+  <si>
+    <t>SSQ-102-03-G-S</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>2N7000</t>
+  </si>
+  <si>
+    <t>R2, R4</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>R7, R9</t>
+  </si>
+  <si>
+    <t>RES 100K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>100K</t>
+  </si>
+  <si>
+    <t>R10, R11</t>
+  </si>
+  <si>
+    <t>MOSFET N-CH 60V 200MA TO92-3</t>
+  </si>
+  <si>
+    <t>TO-92-3</t>
+  </si>
+  <si>
+    <t>onsemi</t>
+  </si>
+  <si>
+    <t>https://rocelec.widen.net/view/pdf/orqxwkxkq1/ONSM-S-A0003544006-1.pdf?t.download=true&amp;u=5oefqw</t>
+  </si>
+  <si>
+    <t>LED GREEN CLEAR 0805 SMD</t>
+  </si>
+  <si>
+    <t>RMCF0805FT100K</t>
+  </si>
+  <si>
+    <t>Stackpole Electronics Inc</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Tahoma"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Tahoma"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -562,10 +664,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="2" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyBorder="1"/>
@@ -577,9 +682,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Comma 2" xfId="3" xr:uid="{93DCE1E9-2D54-4A8D-9F9C-FD11D10FA797}"/>
+    <cellStyle name="Currency 2" xfId="1" xr:uid="{F42CCD68-B275-4B3C-AAD6-BDE77EAD4550}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{5AAD89F3-4562-4E17-9686-908AF945E698}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
@@ -891,10 +1006,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -911,7 +1026,7 @@
     <col min="10" max="10" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -943,7 +1058,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
@@ -975,7 +1090,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>19</v>
       </c>
@@ -1007,7 +1122,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>26</v>
       </c>
@@ -1039,7 +1154,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>31</v>
       </c>
@@ -1071,15 +1186,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B6" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>35</v>
@@ -1094,18 +1209,18 @@
         <v>37</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>38</v>
+        <v>131</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
@@ -1135,15 +1250,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>134</v>
+        <v>38</v>
       </c>
       <c r="B8" s="6">
         <v>1</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>136</v>
+      <c r="C8" s="17" t="s">
+        <v>160</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>35</v>
@@ -1158,16 +1273,16 @@
         <v>37</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>17</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>43</v>
       </c>
@@ -1199,7 +1314,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>50</v>
       </c>
@@ -1231,7 +1346,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>55</v>
       </c>
@@ -1263,274 +1378,282 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" s="3">
+        <v>430251000</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="K12" s="11"/>
+      <c r="M12" s="11"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B13" s="5">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" s="3">
+        <v>430300002</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="K13" s="11"/>
+      <c r="M13" s="11"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="6">
-        <v>1</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="B14" s="6">
+        <v>1</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="I12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J12" s="4" t="s">
+      <c r="I14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="6">
-        <v>1</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="B15" s="6">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G15" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H15" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="I13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="4" t="s">
+      <c r="I15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
+    <row r="16" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B16" s="5">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K16" s="11"/>
+      <c r="M16" s="11"/>
+    </row>
+    <row r="17" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B17" s="5">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K17" s="11"/>
+      <c r="M17" s="11"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B14" s="6">
-        <v>1</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="B18" s="6">
+        <v>1</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F18" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G18" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H18" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="I14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J14" s="4" t="s">
+      <c r="I18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
+    <row r="19" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="B19" s="16">
+        <v>1</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J19" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B15" s="6">
-        <v>1</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="B20" s="6">
+        <v>1</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="B16" s="6">
-        <v>3</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B17" s="6">
-        <v>1</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="B18" s="6">
-        <v>1</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="B19" s="6">
-        <v>1</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="B20" s="6">
-        <v>1</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>66</v>
@@ -1542,7 +1665,7 @@
         <v>15</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>17</v>
@@ -1551,18 +1674,18 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>108</v>
+        <v>150</v>
       </c>
       <c r="B21" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>66</v>
@@ -1574,109 +1697,301 @@
         <v>15</v>
       </c>
       <c r="H21" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="6">
+        <v>1</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="6">
+        <v>1</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B24" s="6">
+        <v>1</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25" s="6">
+        <v>1</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="B26" s="16">
+        <v>2</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="I26" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B27" s="16">
+        <v>2</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="I27" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J27" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" s="6">
+        <v>2</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="I21" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J21" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="8" t="s">
+      <c r="E28" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B22" s="6">
-        <v>2</v>
-      </c>
-      <c r="C22" s="4" t="s">
+      <c r="F28" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G28" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="H28" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="I28" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J28" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="F22" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G22" s="4" t="s">
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="B29" s="6">
+        <v>1</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="I22" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J22" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="8" t="s">
+      <c r="E29" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B23" s="6">
-        <v>1</v>
-      </c>
-      <c r="C23" s="4" t="s">
+      <c r="G29" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="H29" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="I29" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B30" s="6">
+        <v>1</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F23" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
+      <c r="F30" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="B24" s="6">
-        <v>1</v>
-      </c>
-      <c r="C24" s="4" t="s">
+      <c r="G30" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="H30" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="I30" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J30" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>